<commit_message>
Some more numbers. Tab "run2" is currently most interesting. The first person who can identify, based on the chart there, which task ran on which infrastructure, wins a couple of cpu hours.
Note that I need to get more decent bigjob statistics through the troy api.


git-svn-id: file://localhost/tmp/svn2git/svn@6333 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/concurrent.xlsx
+++ b/papers/troy/pstar/perf/interop/concurrent.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16920" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16920" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>Queue</t>
   </si>
@@ -124,6 +124,54 @@
   <si>
     <t>troy.workunit.41b1aa16-1c09-4dcd-bdd3-4e334f4cfcc3</t>
   </si>
+  <si>
+    <t>troy.workunit.fc3b5ddf-19cc-4d17-bd4c-2b3a026cfc1d</t>
+  </si>
+  <si>
+    <t>troy.workunit.de28990e-d2c6-4cf9-a2f9-fed529600aea</t>
+  </si>
+  <si>
+    <t>troy.workunit.0de1c3f4-c6b8-4244-832c-0b6812c3c6b9</t>
+  </si>
+  <si>
+    <t>troy.workunit.68c1b153-6f07-4fe0-94dd-dfa8fd8d236e</t>
+  </si>
+  <si>
+    <t>troy.workunit.9fb5823d-6eb2-4b04-b3c8-b62af921a782</t>
+  </si>
+  <si>
+    <t>troy.workunit.10912201-0707-464a-aea3-3aea91f166f8</t>
+  </si>
+  <si>
+    <t>troy.workunit.fa78ae5a-a899-42c9-820b-56dead71dd78</t>
+  </si>
+  <si>
+    <t>troy.workunit.6297dd5e-568b-49b5-becd-2e8bc7c59cfb</t>
+  </si>
+  <si>
+    <t>troy.workunit.925b252c-7785-4316-b619-aa69060cf042</t>
+  </si>
+  <si>
+    <t>troy.workunit.8c7e4009-f5fe-4f2c-a4ea-2ffb9c4ab039</t>
+  </si>
+  <si>
+    <t>troy.workunit.e8b67d8c-092d-432a-b05b-0fe4c3083415</t>
+  </si>
+  <si>
+    <t>troy.workunit.b38bbb0a-6a8e-450e-a2cd-4961bea5ed2e</t>
+  </si>
+  <si>
+    <t>troy.workunit.407aa122-90ef-41bf-bd27-0dc5f5d289e6</t>
+  </si>
+  <si>
+    <t>troy.workunit.729038f4-6666-4f10-8bc2-f04597fe5c18</t>
+  </si>
+  <si>
+    <t>troy.workunit.50e5faf5-bf9b-49df-b951-a14c8ca2e2da</t>
+  </si>
+  <si>
+    <t>troy.workunit.b8eea7d5-053b-4336-8e97-883eaab12183</t>
+  </si>
 </sst>
 </file>
 
@@ -193,8 +241,90 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -272,7 +402,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="153">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -308,6 +438,47 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -343,6 +514,47 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -419,10 +631,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>27.967966016375</c:v>
+                  <c:v>29.34370227343672</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>15.20084372535547</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -434,7 +646,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.593593203275001</c:v>
+                  <c:v>8.908909199758437</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -491,7 +703,7 @@
                   <c:v>2.747271589945312</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>2.136944891890625</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -503,7 +715,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.549454317989063</c:v>
+                  <c:v>0.976843296367188</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -557,10 +769,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>13.39181710221094</c:v>
+                  <c:v>15.50980202108672</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>14.22107832879297</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -572,7 +784,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.678363420442187</c:v>
+                  <c:v>5.946176069975938</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -631,10 +843,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.01768343709375</c:v>
+                  <c:v>0.52396226115625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0.518845291796874</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -646,7 +858,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.80353668741875</c:v>
+                  <c:v>0.208561510590625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -743,7 +955,7 @@
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Cumulative time of 128 Bfast runs on EGI using DIANE</a:t>
+              <a:t>Cumulative time of 16 Bfast runs on EGI and Future Grid concurrently</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
               <a:effectLst/>
@@ -785,10 +997,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'run1'!$K$2:$K$129</c:f>
+              <c:f>'run1'!$K$2:$K$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="128"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>250.425715923</c:v>
                 </c:pt>
@@ -802,10 +1014,10 @@
                   <c:v>258.4430058</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>58.842881918</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>58.5532259941</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>255.437237978</c:v>
@@ -820,7 +1032,7 @@
                   <c:v>410.667474031</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0</c:v>
+                  <c:v>58.6981329918</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>331.563977957</c:v>
@@ -836,342 +1048,6 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>232.380609989</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1194,10 +1070,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'run1'!$L$2:$L$129</c:f>
+              <c:f>'run1'!$L$2:$L$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="128"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>35.06663703899997</c:v>
                 </c:pt>
@@ -1245,342 +1121,6 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>30.07108283100001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1603,10 +1143,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'run1'!$M$2:$M$129</c:f>
+              <c:f>'run1'!$M$2:$M$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="128"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>120.168606043</c:v>
                 </c:pt>
@@ -1620,10 +1160,10 @@
                   <c:v>120.167285919</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>90.36740589099999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>90.3672928809</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>121.168799877</c:v>
@@ -1638,7 +1178,7 @@
                   <c:v>120.055586815</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0</c:v>
+                  <c:v>90.3673708442</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>120.110852957</c:v>
@@ -1654,342 +1194,6 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>151.220239162</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2012,10 +1216,10 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'run1'!$N$2:$N$129</c:f>
+              <c:f>'run1'!$N$2:$N$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="128"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>5.005764008000028</c:v>
                 </c:pt>
@@ -2029,10 +1233,10 @@
                   <c:v>7.009393214999988</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>149.210287809</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>148.920518875</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7.008949041999983</c:v>
@@ -2047,7 +1251,7 @@
                   <c:v>4.00001096699998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>149.065503836</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>4.00481510100002</c:v>
@@ -2063,342 +1267,6 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>7.007189988999983</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2538,7 +1406,7 @@
               <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Cumulative time of 128 Bfast runs on EGI using DIANE</a:t>
+              <a:t>Cumulative time of 16 Bfast runs on EGI and Future Grid concurrently</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
               <a:effectLst/>
@@ -2580,393 +1448,57 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'run2'!$K$2:$K$129</c:f>
+              <c:f>'run2'!$K$2:$K$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="128"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>55.5747041702</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>128.081809044</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>55.5747041702</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>55.5747041702</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>55.5747041702</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>55.8632881641</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>147.23155117</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0</c:v>
+                  <c:v>132.399979115</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0</c:v>
+                  <c:v>55.5747041702</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0</c:v>
+                  <c:v>202.445611</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0</c:v>
+                  <c:v>310.548897982</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0</c:v>
+                  <c:v>310.548537016</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0</c:v>
+                  <c:v>55.5747041702</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0</c:v>
+                  <c:v>130.096414089</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0</c:v>
+                  <c:v>55.5747041702</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>0.0</c:v>
+                  <c:v>139.468980074</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2989,15 +1521,15 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'run2'!$L$2:$L$129</c:f>
+              <c:f>'run2'!$L$2:$L$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="128"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>37.31995010399999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -3012,370 +1544,34 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>35.19238281300002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0</c:v>
+                  <c:v>40.01060700399998</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0</c:v>
+                  <c:v>14.01457309699998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0</c:v>
+                  <c:v>35.866332054</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0</c:v>
+                  <c:v>31.863518</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0</c:v>
+                  <c:v>38.30923008899998</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>0.0</c:v>
+                  <c:v>40.95235300100001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3398,393 +1594,57 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'run2'!$M$2:$M$129</c:f>
+              <c:f>'run2'!$M$2:$M$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="128"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>85.62101387980001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>140.142369985</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>89.07261991480001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>90.65581393280002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>90.5090608598</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>91.5145049099</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>130.126296997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0</c:v>
+                  <c:v>140.139328003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0</c:v>
+                  <c:v>87.4891278748</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0</c:v>
+                  <c:v>132.957366944</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0</c:v>
+                  <c:v>160.061800957</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0</c:v>
+                  <c:v>130.055958032</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0</c:v>
+                  <c:v>85.7655239108</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0</c:v>
+                  <c:v>150.149518013</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0</c:v>
+                  <c:v>85.9104208948</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>0.0</c:v>
+                  <c:v>130.127300977</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3807,15 +1667,15 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'run2'!$N$2:$N$129</c:f>
+              <c:f>'run2'!$N$2:$N$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="128"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>4.003550052999969</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -3830,370 +1690,34 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>12.85151410100002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0</c:v>
+                  <c:v>13.85193204799998</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0</c:v>
+                  <c:v>4.001091956999971</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0</c:v>
+                  <c:v>4.002047060999985</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0</c:v>
+                  <c:v>4.003054141999996</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0</c:v>
+                  <c:v>10.847882986</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>0.0</c:v>
+                  <c:v>12.851125002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4209,11 +1733,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1119658632"/>
-        <c:axId val="1119664168"/>
+        <c:axId val="904875464"/>
+        <c:axId val="818054136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1119658632"/>
+        <c:axId val="904875464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4241,7 +1765,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1119664168"/>
+        <c:crossAx val="818054136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4249,7 +1773,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1119664168"/>
+        <c:axId val="818054136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4284,7 +1808,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1119658632"/>
+        <c:crossAx val="904875464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9768,19 +7292,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -10235,7 +7759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+    <sheetView topLeftCell="A147" workbookViewId="0">
       <pane ySplit="560" activePane="bottomLeft"/>
       <selection sqref="A1:C147"/>
       <selection pane="bottomLeft" activeCell="L35" sqref="L35"/>
@@ -10269,7 +7793,7 @@
       </c>
       <c r="B2">
         <f>'run1'!$K$130</f>
-        <v>27.967966016375001</v>
+        <v>29.343702273436723</v>
       </c>
       <c r="C2">
         <f>'run1'!$L$130</f>
@@ -10277,15 +7801,15 @@
       </c>
       <c r="D2">
         <f>'run1'!$M$130</f>
-        <v>13.391817102210936</v>
+        <v>15.509802021086717</v>
       </c>
       <c r="E2">
         <f>'run1'!$N$130</f>
-        <v>4.0176834370937495</v>
+        <v>0.52396226115624955</v>
       </c>
       <c r="F2">
         <f>'run1'!$O$130</f>
-        <v>48.124738145625003</v>
+        <v>48.124738145624995</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -10294,23 +7818,23 @@
       </c>
       <c r="B3">
         <f>'run2'!$K$130</f>
-        <v>0</v>
+        <v>15.200843725355469</v>
       </c>
       <c r="C3">
         <f>'run2'!$L$130</f>
-        <v>0</v>
+        <v>2.1369448918906246</v>
       </c>
       <c r="D3">
         <f>'run2'!$M$130</f>
-        <v>0</v>
+        <v>14.221078328792972</v>
       </c>
       <c r="E3">
         <f>'run2'!$N$130</f>
-        <v>0</v>
+        <v>0.51884529179687444</v>
       </c>
       <c r="F3">
         <f>'run2'!$O$130</f>
-        <v>0</v>
+        <v>32.077712237835939</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -10394,23 +7918,23 @@
       </c>
       <c r="B8">
         <f>AVERAGE(B2:B7)</f>
-        <v>5.5935932032750006</v>
+        <v>8.9089091997584369</v>
       </c>
       <c r="C8">
         <f>AVERAGE(C2:C7)</f>
-        <v>0.54945431798906263</v>
+        <v>0.97684329636718759</v>
       </c>
       <c r="D8">
         <f>AVERAGE(D2:D7)</f>
-        <v>2.6783634204421873</v>
+        <v>5.9461760699759383</v>
       </c>
       <c r="E8">
         <f>AVERAGE(E2:E7)</f>
-        <v>0.80353668741874995</v>
+        <v>0.2085615105906248</v>
       </c>
       <c r="F8">
         <f>AVERAGE(F2:F7)</f>
-        <v>9.6249476291249998</v>
+        <v>16.040490076692187</v>
       </c>
     </row>
   </sheetData>
@@ -10429,10 +7953,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O130"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="560" activePane="bottomLeft"/>
       <selection activeCell="K1" sqref="K1:M22"/>
-      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10688,13 +8212,16 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <f>B6</f>
+        <v>58.842881918000003</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <f>B6</f>
+        <v>58.842881918000003</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <f>G6</f>
+        <v>149.21028780899999</v>
       </c>
       <c r="G6">
         <v>149.21028780899999</v>
@@ -10706,20 +8233,20 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>D6</f>
+        <v>58.842881918000003</v>
       </c>
       <c r="L6">
-        <f t="shared" si="1"/>
+        <f>E6-D6</f>
         <v>0</v>
       </c>
       <c r="M6">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>F6-D6</f>
+        <v>90.36740589099999</v>
       </c>
       <c r="N6">
         <f t="shared" si="1"/>
-        <v>149.21028780899999</v>
+        <v>0</v>
       </c>
       <c r="O6">
         <f t="shared" si="2"/>
@@ -10737,13 +8264,16 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <f>B7</f>
+        <v>58.553225994100004</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <f>B7</f>
+        <v>58.553225994100004</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <f>G7</f>
+        <v>148.920518875</v>
       </c>
       <c r="G7">
         <v>148.920518875</v>
@@ -10756,7 +8286,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>58.553225994100004</v>
       </c>
       <c r="L7">
         <f t="shared" si="1"/>
@@ -10764,11 +8294,11 @@
       </c>
       <c r="M7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>90.367292880899996</v>
       </c>
       <c r="N7">
         <f t="shared" si="1"/>
-        <v>148.920518875</v>
+        <v>0</v>
       </c>
       <c r="O7">
         <f t="shared" si="2"/>
@@ -10982,13 +8512,16 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <f>B12</f>
+        <v>58.698132991800001</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <f>B12</f>
+        <v>58.698132991800001</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <f>G12</f>
+        <v>149.065503836</v>
       </c>
       <c r="G12">
         <v>149.065503836</v>
@@ -11001,7 +8534,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>58.698132991800001</v>
       </c>
       <c r="L12">
         <f t="shared" si="1"/>
@@ -11009,11 +8542,11 @@
       </c>
       <c r="M12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>90.367370844199996</v>
       </c>
       <c r="N12">
         <f t="shared" si="1"/>
-        <v>149.065503836</v>
+        <v>0</v>
       </c>
       <c r="O12">
         <f t="shared" si="2"/>
@@ -13739,7 +11272,7 @@
       </c>
       <c r="K130" s="1">
         <f>AVERAGE(K2:K129)</f>
-        <v>27.967966016375001</v>
+        <v>29.343702273436723</v>
       </c>
       <c r="L130" s="1">
         <f>AVERAGE(L2:L129)</f>
@@ -13747,15 +11280,15 @@
       </c>
       <c r="M130" s="1">
         <f>AVERAGE(M2:M129)</f>
-        <v>13.391817102210936</v>
+        <v>15.509802021086717</v>
       </c>
       <c r="N130" s="1">
         <f>AVERAGE(N2:N129)</f>
-        <v>4.0176834370937495</v>
+        <v>0.52396226115624955</v>
       </c>
       <c r="O130" s="1">
         <f>SUM(K130:N130)</f>
-        <v>48.124738145625003</v>
+        <v>48.124738145624995</v>
       </c>
     </row>
   </sheetData>
@@ -13763,6 +11296,9 @@
   <printOptions headings="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="M6" formula="1"/>
+  </ignoredErrors>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -13774,17 +11310,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G1:O130"/>
+  <dimension ref="A1:O130"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J16" workbookViewId="0">
       <pane ySplit="560" activePane="bottomLeft"/>
       <selection activeCell="K1" sqref="K1:M22"/>
-      <selection pane="bottomLeft" activeCell="I129" sqref="A1:I129"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="11:15" s="1" customFormat="1">
+    <row r="1" spans="1:15" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="K1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13801,10 +11364,37 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="11:15">
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2">
+        <v>55.5747041702</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>55.5747041702</v>
+      </c>
+      <c r="E2">
+        <v>55.5747041702</v>
+      </c>
+      <c r="F2">
+        <v>141.19571805000001</v>
+      </c>
+      <c r="G2">
+        <v>141.19571805000001</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
       <c r="K2">
         <f>D2</f>
-        <v>0</v>
+        <v>55.5747041702</v>
       </c>
       <c r="L2">
         <f>E2-D2</f>
@@ -13812,7 +11402,7 @@
       </c>
       <c r="M2">
         <f>F2-E2</f>
-        <v>0</v>
+        <v>85.621013879800017</v>
       </c>
       <c r="N2">
         <f>G2-F2</f>
@@ -13820,35 +11410,89 @@
       </c>
       <c r="O2">
         <f>SUM(K2:N2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="11:15">
+        <v>141.19571805000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3">
+        <v>55.5747041702</v>
+      </c>
+      <c r="C3">
+        <v>54.853811025600002</v>
+      </c>
+      <c r="D3">
+        <v>128.08180904400001</v>
+      </c>
+      <c r="E3">
+        <v>165.401759148</v>
+      </c>
+      <c r="F3">
+        <v>305.54412913300001</v>
+      </c>
+      <c r="G3">
+        <v>309.54767918599998</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
       <c r="K3">
         <f t="shared" ref="K3:K66" si="0">D3</f>
-        <v>0</v>
+        <v>128.08180904400001</v>
       </c>
       <c r="L3">
         <f t="shared" ref="L3:N66" si="1">E3-D3</f>
-        <v>0</v>
+        <v>37.319950103999986</v>
       </c>
       <c r="M3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>140.14236998500002</v>
       </c>
       <c r="N3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.0035500529999695</v>
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O66" si="2">SUM(K3:N3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="11:15">
+        <v>309.54767918599998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>55.5747041702</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>55.5747041702</v>
+      </c>
+      <c r="E4">
+        <v>55.5747041702</v>
+      </c>
+      <c r="F4">
+        <v>144.64732408500001</v>
+      </c>
+      <c r="G4">
+        <v>144.64732408500001</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55.5747041702</v>
       </c>
       <c r="L4">
         <f t="shared" si="1"/>
@@ -13856,7 +11500,7 @@
       </c>
       <c r="M4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>89.072619914800015</v>
       </c>
       <c r="N4">
         <f t="shared" si="1"/>
@@ -13864,13 +11508,40 @@
       </c>
       <c r="O4">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="11:15">
+        <v>144.64732408500001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5">
+        <v>55.5747041702</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>55.5747041702</v>
+      </c>
+      <c r="E5">
+        <v>55.5747041702</v>
+      </c>
+      <c r="F5">
+        <v>146.23051810300001</v>
+      </c>
+      <c r="G5">
+        <v>146.23051810300001</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55.5747041702</v>
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
@@ -13878,7 +11549,7 @@
       </c>
       <c r="M5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>90.655813932800015</v>
       </c>
       <c r="N5">
         <f t="shared" si="1"/>
@@ -13886,13 +11557,40 @@
       </c>
       <c r="O5">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="11:15">
+        <v>146.23051810300001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>55.5747041702</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>55.5747041702</v>
+      </c>
+      <c r="E6" s="3">
+        <v>55.5747041702</v>
+      </c>
+      <c r="F6">
+        <v>146.08376503</v>
+      </c>
+      <c r="G6">
+        <v>146.08376503</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55.5747041702</v>
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
@@ -13900,7 +11598,7 @@
       </c>
       <c r="M6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>90.509060859800002</v>
       </c>
       <c r="N6">
         <f t="shared" si="1"/>
@@ -13908,13 +11606,40 @@
       </c>
       <c r="O6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="11:15">
+        <v>146.08376503</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7">
+        <v>55.5747041702</v>
+      </c>
+      <c r="C7">
+        <v>55.863288164099998</v>
+      </c>
+      <c r="D7">
+        <v>55.863288164099998</v>
+      </c>
+      <c r="E7">
+        <v>55.863288164099998</v>
+      </c>
+      <c r="F7">
+        <v>147.37779307400001</v>
+      </c>
+      <c r="G7">
+        <v>147.37779307400001</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55.863288164099998</v>
       </c>
       <c r="L7">
         <f t="shared" si="1"/>
@@ -13922,7 +11647,7 @@
       </c>
       <c r="M7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>91.514504909900012</v>
       </c>
       <c r="N7">
         <f t="shared" si="1"/>
@@ -13930,57 +11655,138 @@
       </c>
       <c r="O7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="11:15">
+        <v>147.37779307400001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8">
+        <v>55.5747041702</v>
+      </c>
+      <c r="C8">
+        <v>64.189484119400007</v>
+      </c>
+      <c r="D8">
+        <v>147.23155116999999</v>
+      </c>
+      <c r="E8">
+        <v>182.42393398300001</v>
+      </c>
+      <c r="F8">
+        <v>312.55023097999998</v>
+      </c>
+      <c r="G8">
+        <v>325.401745081</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>147.23155116999999</v>
       </c>
       <c r="L8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>35.192382813000023</v>
       </c>
       <c r="M8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>130.12629699699997</v>
       </c>
       <c r="N8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12.851514101000021</v>
       </c>
       <c r="O8">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="11:15">
+        <v>325.401745081</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9">
+        <v>55.5747041702</v>
+      </c>
+      <c r="C9">
+        <v>54.853667974499999</v>
+      </c>
+      <c r="D9">
+        <v>132.39997911500001</v>
+      </c>
+      <c r="E9">
+        <v>172.41058611899999</v>
+      </c>
+      <c r="F9">
+        <v>312.54991412200002</v>
+      </c>
+      <c r="G9">
+        <v>326.40184617</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>132.39997911500001</v>
       </c>
       <c r="L9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>40.010607003999979</v>
       </c>
       <c r="M9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>140.13932800300003</v>
       </c>
       <c r="N9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13.851932047999981</v>
       </c>
       <c r="O9">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="11:15">
+        <v>326.40184617</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10">
+        <v>55.5747041702</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>55.5747041702</v>
+      </c>
+      <c r="E10">
+        <v>55.5747041702</v>
+      </c>
+      <c r="F10">
+        <v>143.063832045</v>
+      </c>
+      <c r="G10">
+        <v>143.063832045</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55.5747041702</v>
       </c>
       <c r="L10">
         <f t="shared" si="1"/>
@@ -13988,7 +11794,7 @@
       </c>
       <c r="M10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>87.489127874800005</v>
       </c>
       <c r="N10">
         <f t="shared" si="1"/>
@@ -13996,79 +11802,187 @@
       </c>
       <c r="O10">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="11:15">
+        <v>143.063832045</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11">
+        <v>55.574971198999997</v>
+      </c>
+      <c r="C11">
+        <v>64.189808130299994</v>
+      </c>
+      <c r="D11">
+        <v>202.44561100000001</v>
+      </c>
+      <c r="E11">
+        <v>216.460184097</v>
+      </c>
+      <c r="F11">
+        <v>349.41755104100002</v>
+      </c>
+      <c r="G11">
+        <v>353.418642998</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>202.44561100000001</v>
       </c>
       <c r="L11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>14.014573096999982</v>
       </c>
       <c r="M11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>132.95736694400003</v>
       </c>
       <c r="N11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.0010919569999714</v>
       </c>
       <c r="O11">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="11:15">
+        <v>353.418642998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12">
+        <v>55.574818134300003</v>
+      </c>
+      <c r="C12">
+        <v>64.189653158200002</v>
+      </c>
+      <c r="D12">
+        <v>310.54889798200003</v>
+      </c>
+      <c r="E12">
+        <v>346.41523003600003</v>
+      </c>
+      <c r="F12">
+        <v>506.47703099300003</v>
+      </c>
+      <c r="G12">
+        <v>510.47907805400001</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>310.54889798200003</v>
       </c>
       <c r="L12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>35.866332053999997</v>
       </c>
       <c r="M12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>160.061800957</v>
       </c>
       <c r="N12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.0020470609999848</v>
       </c>
       <c r="O12">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="11:15">
+        <v>510.47907805400001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13">
+        <v>55.430355071999998</v>
+      </c>
+      <c r="C13">
+        <v>64.044972181299997</v>
+      </c>
+      <c r="D13">
+        <v>310.54853701600001</v>
+      </c>
+      <c r="E13">
+        <v>342.41205501600001</v>
+      </c>
+      <c r="F13">
+        <v>472.46801304799999</v>
+      </c>
+      <c r="G13">
+        <v>476.47106718999999</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>310.54853701600001</v>
       </c>
       <c r="L13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>31.863517999999999</v>
       </c>
       <c r="M13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>130.05595803199998</v>
       </c>
       <c r="N13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.0030541419999963</v>
       </c>
       <c r="O13">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="11:15">
+        <v>476.47106718999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14">
+        <v>55.5747041702</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>55.5747041702</v>
+      </c>
+      <c r="E14">
+        <v>55.5747041702</v>
+      </c>
+      <c r="F14">
+        <v>141.34022808099999</v>
+      </c>
+      <c r="G14">
+        <v>141.34022808099999</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55.5747041702</v>
       </c>
       <c r="L14">
         <f t="shared" si="1"/>
@@ -14076,7 +11990,7 @@
       </c>
       <c r="M14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>85.765523910799999</v>
       </c>
       <c r="N14">
         <f t="shared" si="1"/>
@@ -14084,35 +11998,89 @@
       </c>
       <c r="O14">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="11:15">
+        <v>141.34022808099999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15">
+        <v>55.5747041702</v>
+      </c>
+      <c r="C15">
+        <v>54.709284067200002</v>
+      </c>
+      <c r="D15">
+        <v>130.09641408900001</v>
+      </c>
+      <c r="E15">
+        <v>168.40564417799999</v>
+      </c>
+      <c r="F15">
+        <v>318.55516219100002</v>
+      </c>
+      <c r="G15">
+        <v>329.40304517700002</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>130.09641408900001</v>
       </c>
       <c r="L15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>38.309230088999982</v>
       </c>
       <c r="M15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>150.14951801300003</v>
       </c>
       <c r="N15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10.847882986000002</v>
       </c>
       <c r="O15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="11:15">
+        <v>329.40304517700002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16">
+        <v>55.5747041702</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>55.5747041702</v>
+      </c>
+      <c r="E16">
+        <v>55.5747041702</v>
+      </c>
+      <c r="F16">
+        <v>141.48512506500001</v>
+      </c>
+      <c r="G16">
+        <v>141.48512506500001</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55.5747041702</v>
       </c>
       <c r="L16">
         <f t="shared" si="1"/>
@@ -14120,7 +12088,7 @@
       </c>
       <c r="M16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>85.910420894800012</v>
       </c>
       <c r="N16">
         <f t="shared" si="1"/>
@@ -14128,32 +12096,59 @@
       </c>
       <c r="O16">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="11:15">
+        <v>141.48512506500001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17">
+        <v>55.430489063300001</v>
+      </c>
+      <c r="C17">
+        <v>64.045156001999999</v>
+      </c>
+      <c r="D17">
+        <v>139.468980074</v>
+      </c>
+      <c r="E17">
+        <v>180.42133307500001</v>
+      </c>
+      <c r="F17">
+        <v>310.54863405200001</v>
+      </c>
+      <c r="G17">
+        <v>323.39975905400001</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>139.468980074</v>
       </c>
       <c r="L17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>40.952353001000006</v>
       </c>
       <c r="M17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>130.127300977</v>
       </c>
       <c r="N17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12.851125002000003</v>
       </c>
       <c r="O17">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="11:15">
+        <v>323.39975905400001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="K18">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -14175,7 +12170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="11:15">
+    <row r="19" spans="1:15">
       <c r="K19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -14197,7 +12192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="11:15">
+    <row r="20" spans="1:15">
       <c r="K20">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -14219,7 +12214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="11:15">
+    <row r="21" spans="1:15">
       <c r="K21">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -14241,7 +12236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="11:15">
+    <row r="22" spans="1:15">
       <c r="K22">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -14263,7 +12258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="11:15">
+    <row r="23" spans="1:15">
       <c r="K23">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -14285,7 +12280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="11:15">
+    <row r="24" spans="1:15">
       <c r="K24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -14307,7 +12302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="11:15">
+    <row r="25" spans="1:15">
       <c r="K25">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -14329,7 +12324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="11:15">
+    <row r="26" spans="1:15">
       <c r="K26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -14351,7 +12346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="11:15">
+    <row r="27" spans="1:15">
       <c r="K27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -14373,7 +12368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="11:15">
+    <row r="28" spans="1:15">
       <c r="K28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -14395,7 +12390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="11:15">
+    <row r="29" spans="1:15">
       <c r="K29">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -14417,7 +12412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="11:15">
+    <row r="30" spans="1:15">
       <c r="K30">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -14439,7 +12434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="11:15">
+    <row r="31" spans="1:15">
       <c r="K31">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -14461,7 +12456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="11:15">
+    <row r="32" spans="1:15">
       <c r="K32">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -16618,32 +14613,32 @@
       </c>
     </row>
     <row r="130" spans="7:15">
-      <c r="G130" s="1" t="e">
+      <c r="G130" s="1">
         <f>AVERAGE(G2:G129)</f>
-        <v>#DIV/0!</v>
+        <v>256.62169790268752</v>
       </c>
       <c r="J130" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K130" s="1">
         <f>AVERAGE(K2:K129)</f>
-        <v>0</v>
+        <v>15.200843725355469</v>
       </c>
       <c r="L130" s="1">
         <f>AVERAGE(L2:L129)</f>
-        <v>0</v>
+        <v>2.1369448918906246</v>
       </c>
       <c r="M130" s="1">
         <f>AVERAGE(M2:M129)</f>
-        <v>0</v>
+        <v>14.221078328792972</v>
       </c>
       <c r="N130" s="1">
         <f>AVERAGE(N2:N129)</f>
-        <v>0</v>
+        <v>0.51884529179687444</v>
       </c>
       <c r="O130" s="1">
         <f>SUM(K130:N130)</f>
-        <v>0</v>
+        <v>32.077712237835939</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added detailed summary statistics.
git-svn-id: file://localhost/tmp/svn2git/svn@6441 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/concurrent.xlsx
+++ b/papers/troy/pstar/perf/interop/concurrent.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="914">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="915">
   <si>
     <t>Queue</t>
   </si>
@@ -2773,6 +2773,9 @@
   </si>
   <si>
     <t>BIGJOB</t>
+  </si>
+  <si>
+    <t>FG</t>
   </si>
 </sst>
 </file>
@@ -2850,8 +2853,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="409">
+  <cellStyleXfs count="439">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3268,7 +3301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="409">
+  <cellStyles count="439">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3473,6 +3506,21 @@
     <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3677,6 +3725,21 @@
     <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -17796,16 +17859,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>165106</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152406</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18593,17 +18656,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
       <pane ySplit="560" activePane="bottomLeft"/>
       <selection sqref="A1:C147"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -18616,7 +18679,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -18629,7 +18692,7 @@
         <v>1212.8018984285716</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -18642,7 +18705,7 @@
         <v>1254.3317010400001</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -18655,7 +18718,7 @@
         <v>2148.8040556623728</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -18668,7 +18731,7 @@
         <v>1091.8222408393551</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -18681,7 +18744,7 @@
         <v>1194.1639064690908</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -18692,6 +18755,246 @@
       <c r="C8">
         <f>AVERAGE(C2:C7)</f>
         <v>1380.3847604878779</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15">
+        <v>396.8382733071287</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>815.96362512144287</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1212.8018984285716</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16">
+        <v>402.09540353915372</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>855.65146490669247</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1254.3317010400001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="B17">
+        <v>320.74402745296607</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1828.0600282094067</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>2148.8040556623728</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="B18">
+        <v>315.48696238203331</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>776.33527845732181</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1091.8222408393551</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="B19">
+        <v>363.53048029093935</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>830.63342617815135</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1194.1639064690908</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="B20" s="1">
+        <f>AVERAGE(B15:B19)</f>
+        <v>359.73902939444417</v>
+      </c>
+      <c r="C20" s="1">
+        <f>AVERAGE(C15:C19)</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <f>AVERAGE(D15:D19)</f>
+        <v>1021.3287645746029</v>
+      </c>
+      <c r="E20" s="1">
+        <f>AVERAGE(E15:E19)</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <f>AVERAGE(F15:F19)</f>
+        <v>1380.3847604878779</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="B22">
+        <v>451.8414150312413</v>
+      </c>
+      <c r="C22">
+        <v>2979.7817796961717</v>
+      </c>
+      <c r="D22">
+        <v>811.8439595537933</v>
+      </c>
+      <c r="E22">
+        <v>4.9106052455172726</v>
+      </c>
+      <c r="F22">
+        <v>4243.4671542812066</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="B23">
+        <v>845.18556271249201</v>
+      </c>
+      <c r="C23">
+        <v>3009.6137638619521</v>
+      </c>
+      <c r="D23">
+        <v>853.06045265488922</v>
+      </c>
+      <c r="E23">
+        <v>36.829210205714318</v>
+      </c>
+      <c r="F23">
+        <v>4707.8597792293331</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="B24">
+        <v>1685.4928219769567</v>
+      </c>
+      <c r="C24">
+        <v>1343.132933982899</v>
+      </c>
+      <c r="D24">
+        <v>850.85122404608717</v>
+      </c>
+      <c r="E24">
+        <v>35.35243507695651</v>
+      </c>
+      <c r="F24">
+        <v>3879.476980005943</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="B25">
+        <v>742.82642156635939</v>
+      </c>
+      <c r="C25">
+        <v>3106.7414845002049</v>
+      </c>
+      <c r="D25">
+        <v>872.95028274156243</v>
+      </c>
+      <c r="E25">
+        <v>23.330915592031175</v>
+      </c>
+      <c r="F25">
+        <v>4722.518188808127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="B26">
+        <v>408.34523463643563</v>
+      </c>
+      <c r="C26">
+        <v>3083.8557407830767</v>
+      </c>
+      <c r="D26">
+        <v>813.916388522121</v>
+      </c>
+      <c r="E26">
+        <v>15.558405373986883</v>
+      </c>
+      <c r="F26">
+        <v>4306.1173639416338</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B27" s="1">
+        <f>AVERAGE(B22:B26)</f>
+        <v>826.73829118469689</v>
+      </c>
+      <c r="C27" s="1">
+        <f>AVERAGE(C22:C26)</f>
+        <v>2704.6251405648609</v>
+      </c>
+      <c r="D27" s="1">
+        <f>AVERAGE(D22:D26)</f>
+        <v>840.52446150369065</v>
+      </c>
+      <c r="E27" s="1">
+        <f>AVERAGE(E22:E26)</f>
+        <v>23.196314298841234</v>
+      </c>
+      <c r="F27" s="1">
+        <f>AVERAGE(F22:F26)</f>
+        <v>4371.8878932532489</v>
       </c>
     </row>
   </sheetData>
@@ -35122,8 +35425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O131"/>
   <sheetViews>
-    <sheetView topLeftCell="E92" workbookViewId="0">
-      <selection activeCell="O131" sqref="O131"/>
+    <sheetView topLeftCell="E111" workbookViewId="0">
+      <selection activeCell="K131" sqref="K131:O131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -41523,8 +41826,8 @@
   <dimension ref="A1:O131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1:O1"/>
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K131" sqref="K131:O131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -47923,9 +48226,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O131"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1:O1"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K131" sqref="K131:O131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -54332,8 +54635,8 @@
   <dimension ref="A1:O127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O127" sqref="O127"/>
+      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K127" sqref="K127:O127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -60545,8 +60848,8 @@
   <dimension ref="A1:O131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O131" sqref="O131"/>
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K131" sqref="K131:O131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>